<commit_message>
planning en takenverdeling aangepast
</commit_message>
<xml_diff>
--- a/CoolTeam_Planning.xlsx
+++ b/CoolTeam_Planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manoelledeviron/Documents/KUL/2020-2021/IoT Nodes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manoelledeviron/Documents/KUL/2020-2021/IoT Nodes/Labo/CoolTeam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD34A92-2936-4E41-ACE2-E0689B15FBC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77FAA20-30DC-334F-BF2D-F9E803797A06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{9C5B68C6-FA56-0F40-BC7E-BD3216375431}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9C5B68C6-FA56-0F40-BC7E-BD3216375431}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>Week 1</t>
   </si>
@@ -116,12 +116,6 @@
     <t>PCBs + BOM PCB's</t>
   </si>
   <si>
-    <t>Solderen + testen PCBs, programmeren</t>
-  </si>
-  <si>
-    <t>Initiële testen finaal product</t>
-  </si>
-  <si>
     <t>Finale: field-testen + presentatie</t>
   </si>
   <si>
@@ -267,13 +261,22 @@
   </si>
   <si>
     <t>werken aan labo: testen van LoRa, Hall en temp sensor</t>
+  </si>
+  <si>
+    <t>Solderen + testen PCBs, programmeren + Initiële testen finaal product?</t>
+  </si>
+  <si>
+    <t>Solderen + testen PCBs, programmeren?</t>
+  </si>
+  <si>
+    <t>testen van GPS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -294,6 +297,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -303,7 +313,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -391,11 +401,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF4472C4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -428,6 +447,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -824,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699C4EC0-9B2F-1A4B-AD6D-4FAF1C0387E4}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -861,7 +883,7 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -890,7 +912,7 @@
         <v>44248</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -901,13 +923,13 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="120" thickBot="1" x14ac:dyDescent="0.25">
@@ -924,7 +946,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="10"/>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1119,12 +1141,14 @@
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1177,7 +1201,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1209,30 +1233,28 @@
         <v>44290</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="B22" s="1"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="10"/>
@@ -1375,11 +1397,13 @@
       <c r="G30" s="7"/>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1425,12 +1449,12 @@
       <c r="G33" s="7"/>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:8" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="154" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1520,7 +1544,7 @@
         <v>20</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1534,7 +1558,7 @@
         <v>21</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1556,7 +1580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9D8C9C-485B-B449-A56F-75DC0666C2B4}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -1568,199 +1592,199 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1788,21 +1812,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1810,10 +1834,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1821,10 +1845,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
         <v>66</v>
-      </c>
-      <c r="B4" t="s">
-        <v>68</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1832,10 +1856,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1843,10 +1867,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1854,10 +1878,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7">
         <v>1</v>

</xml_diff>